<commit_message>
added extra feature to sort/print by stat
</commit_message>
<xml_diff>
--- a/stats.xlsx
+++ b/stats.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rbrewster\Documents\teks\ExcelReader\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EDD9441-BE91-4E02-8EFE-473325248673}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35105EA7-010D-4900-B54E-BDB74E708421}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{F658C51F-30AF-4D3C-9AFE-D9E6A599C11D}"/>
+    <workbookView xWindow="-28920" yWindow="-1665" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{F658C51F-30AF-4D3C-9AFE-D9E6A599C11D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -489,22 +489,22 @@
         <v>1</v>
       </c>
       <c r="B1" s="2">
-        <v>493</v>
+        <v>677</v>
       </c>
       <c r="C1" s="2">
-        <v>160</v>
+        <v>216</v>
       </c>
       <c r="D1" s="2">
-        <v>516</v>
+        <v>720</v>
       </c>
       <c r="E1" s="2">
-        <v>49</v>
+        <v>64</v>
       </c>
       <c r="F1" s="2">
-        <v>0.26900000000000002</v>
+        <v>0.26500000000000001</v>
       </c>
       <c r="G1" s="2">
-        <v>0.80700000000000005</v>
+        <v>0.79600000000000004</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
@@ -512,22 +512,22 @@
         <v>3</v>
       </c>
       <c r="B2" s="2">
-        <v>550</v>
+        <v>741</v>
       </c>
       <c r="C2" s="2">
-        <v>152</v>
+        <v>212</v>
       </c>
       <c r="D2" s="2">
-        <v>508</v>
+        <v>699</v>
       </c>
       <c r="E2" s="2">
-        <v>63</v>
+        <v>72</v>
       </c>
       <c r="F2" s="2">
         <v>0.25</v>
       </c>
       <c r="G2" s="2">
-        <v>0.78700000000000003</v>
+        <v>0.78600000000000003</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -535,22 +535,22 @@
         <v>2</v>
       </c>
       <c r="B3" s="2">
-        <v>509</v>
+        <v>734</v>
       </c>
       <c r="C3" s="2">
-        <v>138</v>
+        <v>188</v>
       </c>
       <c r="D3" s="2">
-        <v>487</v>
+        <v>677</v>
       </c>
       <c r="E3" s="2">
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="F3" s="2">
-        <v>0.24099999999999999</v>
+        <v>0.245</v>
       </c>
       <c r="G3" s="2">
-        <v>0.73399999999999999</v>
+        <v>0.74</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="44" thickBot="1" x14ac:dyDescent="0.4">
@@ -558,22 +558,22 @@
         <v>4</v>
       </c>
       <c r="B4" s="2">
-        <v>432</v>
+        <v>631</v>
       </c>
       <c r="C4" s="2">
-        <v>117</v>
+        <v>173</v>
       </c>
       <c r="D4" s="2">
-        <v>444</v>
+        <v>611</v>
       </c>
       <c r="E4" s="2">
-        <v>60</v>
+        <v>87</v>
       </c>
       <c r="F4" s="2">
-        <v>0.253</v>
+        <v>0.25700000000000001</v>
       </c>
       <c r="G4" s="2">
-        <v>0.75</v>
+        <v>0.76</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
@@ -581,22 +581,22 @@
         <v>5</v>
       </c>
       <c r="B5" s="2">
-        <v>539</v>
+        <v>724</v>
       </c>
       <c r="C5" s="2">
-        <v>156</v>
+        <v>208</v>
       </c>
       <c r="D5" s="2">
-        <v>499</v>
+        <v>674</v>
       </c>
       <c r="E5" s="2">
-        <v>54</v>
+        <v>75</v>
       </c>
       <c r="F5" s="2">
-        <v>0.26700000000000002</v>
+        <v>0.26500000000000001</v>
       </c>
       <c r="G5" s="2">
-        <v>0.82099999999999995</v>
+        <v>0.81399999999999995</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
@@ -604,22 +604,22 @@
         <v>6</v>
       </c>
       <c r="B6" s="2">
-        <v>492</v>
+        <v>670</v>
       </c>
       <c r="C6" s="2">
-        <v>118</v>
+        <v>158</v>
       </c>
       <c r="D6" s="2">
-        <v>423</v>
+        <v>587</v>
       </c>
       <c r="E6" s="2">
-        <v>66</v>
+        <v>106</v>
       </c>
       <c r="F6" s="2">
-        <v>0.26400000000000001</v>
+        <v>0.26800000000000002</v>
       </c>
       <c r="G6" s="2">
-        <v>0.76800000000000002</v>
+        <v>0.77200000000000002</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
@@ -627,22 +627,22 @@
         <v>7</v>
       </c>
       <c r="B7" s="2">
-        <v>506</v>
+        <v>720</v>
       </c>
       <c r="C7" s="2">
-        <v>145</v>
+        <v>209</v>
       </c>
       <c r="D7" s="2">
-        <v>483</v>
+        <v>686</v>
       </c>
       <c r="E7" s="2">
-        <v>69</v>
+        <v>91</v>
       </c>
       <c r="F7" s="2">
-        <v>0.251</v>
+        <v>0.25600000000000001</v>
       </c>
       <c r="G7" s="2">
-        <v>0.76200000000000001</v>
+        <v>0.77600000000000002</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
@@ -650,22 +650,22 @@
         <v>0</v>
       </c>
       <c r="B8" s="4">
-        <v>551</v>
+        <v>786</v>
       </c>
       <c r="C8" s="4">
-        <v>151</v>
+        <v>232</v>
       </c>
       <c r="D8" s="4">
-        <v>507</v>
+        <v>739</v>
       </c>
       <c r="E8" s="4">
-        <v>62</v>
+        <v>82</v>
       </c>
       <c r="F8" s="4">
-        <v>0.25700000000000001</v>
+        <v>0.26100000000000001</v>
       </c>
       <c r="G8" s="4">
-        <v>0.79</v>
+        <v>0.80900000000000005</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
@@ -673,22 +673,22 @@
         <v>8</v>
       </c>
       <c r="B9" s="2">
-        <v>498</v>
+        <v>696</v>
       </c>
       <c r="C9" s="2">
-        <v>145</v>
+        <v>205</v>
       </c>
       <c r="D9" s="2">
-        <v>470</v>
+        <v>659</v>
       </c>
       <c r="E9" s="2">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="F9" s="2">
-        <v>0.26</v>
+        <v>0.26400000000000001</v>
       </c>
       <c r="G9" s="2">
-        <v>0.79100000000000004</v>
+        <v>0.80200000000000005</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
@@ -696,22 +696,22 @@
         <v>9</v>
       </c>
       <c r="B10" s="2">
-        <v>538</v>
+        <v>736</v>
       </c>
       <c r="C10" s="2">
-        <v>126</v>
+        <v>184</v>
       </c>
       <c r="D10" s="2">
-        <v>469</v>
+        <v>640</v>
       </c>
       <c r="E10" s="2">
-        <v>61</v>
+        <v>77</v>
       </c>
       <c r="F10" s="2">
-        <v>0.25600000000000001</v>
+        <v>0.25900000000000001</v>
       </c>
       <c r="G10" s="2">
-        <v>0.751</v>
+        <v>0.76600000000000001</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="58.5" thickBot="1" x14ac:dyDescent="0.4">
@@ -719,22 +719,22 @@
         <v>10</v>
       </c>
       <c r="B11" s="2">
-        <v>499</v>
+        <v>720</v>
       </c>
       <c r="C11" s="2">
-        <v>164</v>
+        <v>241</v>
       </c>
       <c r="D11" s="2">
-        <v>476</v>
+        <v>680</v>
       </c>
       <c r="E11" s="2">
-        <v>44</v>
+        <v>58</v>
       </c>
       <c r="F11" s="2">
-        <v>0.254</v>
+        <v>0.25700000000000001</v>
       </c>
       <c r="G11" s="2">
-        <v>0.79700000000000004</v>
+        <v>0.80900000000000005</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
@@ -742,22 +742,22 @@
         <v>11</v>
       </c>
       <c r="B12" s="2">
-        <v>534</v>
+        <v>732</v>
       </c>
       <c r="C12" s="2">
-        <v>156</v>
+        <v>222</v>
       </c>
       <c r="D12" s="2">
-        <v>510</v>
+        <v>723</v>
       </c>
       <c r="E12" s="2">
-        <v>55</v>
+        <v>76</v>
       </c>
       <c r="F12" s="2">
-        <v>0.25900000000000001</v>
+        <v>0.26100000000000001</v>
       </c>
       <c r="G12" s="2">
-        <v>0.79100000000000004</v>
+        <v>0.79200000000000004</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -765,22 +765,22 @@
         <v>12</v>
       </c>
       <c r="B13" s="2">
-        <v>520</v>
+        <v>728</v>
       </c>
       <c r="C13" s="2">
-        <v>160</v>
+        <v>209</v>
       </c>
       <c r="D13" s="2">
-        <v>561</v>
+        <v>746</v>
       </c>
       <c r="E13" s="2">
-        <v>73</v>
+        <v>99</v>
       </c>
       <c r="F13" s="2">
-        <v>0.253</v>
+        <v>0.25800000000000001</v>
       </c>
       <c r="G13" s="2">
-        <v>0.76500000000000001</v>
+        <v>0.77600000000000002</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
@@ -788,19 +788,19 @@
         <v>13</v>
       </c>
       <c r="B14" s="2">
-        <v>530</v>
+        <v>718</v>
       </c>
       <c r="C14" s="2">
-        <v>182</v>
+        <v>254</v>
       </c>
       <c r="D14" s="2">
-        <v>546</v>
+        <v>755</v>
       </c>
       <c r="E14" s="2">
-        <v>50</v>
+        <v>58</v>
       </c>
       <c r="F14" s="2">
-        <v>0.254</v>
+        <v>0.25</v>
       </c>
       <c r="G14" s="2">
         <v>0.79900000000000004</v>
@@ -808,20 +808,20 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A1" r:id="rId1" display="https://baseball.fantasysports.yahoo.com/b1/29905/1" xr:uid="{706AD5E4-4E22-4E39-80F0-410D37103B22}"/>
-    <hyperlink ref="A2" r:id="rId2" display="https://baseball.fantasysports.yahoo.com/b1/29905/3" xr:uid="{64F36E41-ADC0-4FD7-90A8-06B958B647B3}"/>
-    <hyperlink ref="A3" r:id="rId3" display="https://baseball.fantasysports.yahoo.com/b1/29905/4" xr:uid="{65A9D5BF-1A30-4270-961D-BC62391F58C8}"/>
-    <hyperlink ref="A4" r:id="rId4" display="https://baseball.fantasysports.yahoo.com/b1/29905/5" xr:uid="{F20D411C-4F80-4EB2-9745-9B9EF948525B}"/>
-    <hyperlink ref="A5" r:id="rId5" display="https://baseball.fantasysports.yahoo.com/b1/29905/6" xr:uid="{78A5233D-52CE-43D8-9237-545AAD2223B8}"/>
-    <hyperlink ref="A6" r:id="rId6" display="https://baseball.fantasysports.yahoo.com/b1/29905/7" xr:uid="{444B4A9B-95A3-4265-B978-38DAAA7E5F38}"/>
-    <hyperlink ref="A7" r:id="rId7" display="https://baseball.fantasysports.yahoo.com/b1/29905/8" xr:uid="{5D3631C5-5C83-469B-9D9E-7CD28E8A358A}"/>
-    <hyperlink ref="A8" r:id="rId8" display="https://baseball.fantasysports.yahoo.com/b1/29905/9" xr:uid="{2DA6A2A5-A511-45CB-8C7C-9FC8C57D2DE2}"/>
-    <hyperlink ref="A9" r:id="rId9" display="https://baseball.fantasysports.yahoo.com/b1/29905/10" xr:uid="{716C37E1-A3A8-4DE7-8E12-1A869C914E22}"/>
-    <hyperlink ref="A10" r:id="rId10" display="https://baseball.fantasysports.yahoo.com/b1/29905/11" xr:uid="{BFC15A98-D0A1-4B20-B493-C3F564E8CBBE}"/>
-    <hyperlink ref="A11" r:id="rId11" display="https://baseball.fantasysports.yahoo.com/b1/29905/12" xr:uid="{5E7128D5-EA5E-4CB6-8BBF-7B20521BCB88}"/>
-    <hyperlink ref="A12" r:id="rId12" display="https://baseball.fantasysports.yahoo.com/b1/29905/13" xr:uid="{DE6CA4DB-3C8E-4264-A8B0-691A4DDD8108}"/>
-    <hyperlink ref="A13" r:id="rId13" display="https://baseball.fantasysports.yahoo.com/b1/29905/14" xr:uid="{BED2D158-128F-4095-B126-50F67FB7E4EA}"/>
-    <hyperlink ref="A14" r:id="rId14" display="https://baseball.fantasysports.yahoo.com/b1/29905/15" xr:uid="{0A9049B4-3EDE-40D7-A3FF-8F5707F68D6D}"/>
+    <hyperlink ref="A1" r:id="rId1" display="https://baseball.fantasysports.yahoo.com/b1/29905/1" xr:uid="{698A05E0-A0E5-4AAA-9023-9AA4089B59F0}"/>
+    <hyperlink ref="A2" r:id="rId2" display="https://baseball.fantasysports.yahoo.com/b1/29905/3" xr:uid="{DF63C015-F062-4C14-948A-40939370E69C}"/>
+    <hyperlink ref="A3" r:id="rId3" display="https://baseball.fantasysports.yahoo.com/b1/29905/4" xr:uid="{4DEE6337-E3A0-4DB5-83EE-12EBFA20E4A4}"/>
+    <hyperlink ref="A4" r:id="rId4" display="https://baseball.fantasysports.yahoo.com/b1/29905/5" xr:uid="{579BB48F-3065-45F3-B51D-E964BA33B5FE}"/>
+    <hyperlink ref="A5" r:id="rId5" display="https://baseball.fantasysports.yahoo.com/b1/29905/6" xr:uid="{E7992124-FED2-4A2A-820A-97075494C75A}"/>
+    <hyperlink ref="A6" r:id="rId6" display="https://baseball.fantasysports.yahoo.com/b1/29905/7" xr:uid="{9E2C6DC8-ED11-44BA-B5F3-D3EAC4F2DF51}"/>
+    <hyperlink ref="A7" r:id="rId7" display="https://baseball.fantasysports.yahoo.com/b1/29905/8" xr:uid="{F4230918-7E82-44B5-9A3D-9BA035B2FABA}"/>
+    <hyperlink ref="A8" r:id="rId8" display="https://baseball.fantasysports.yahoo.com/b1/29905/9" xr:uid="{795E5BE4-38F1-4222-9C73-725061D632B1}"/>
+    <hyperlink ref="A9" r:id="rId9" display="https://baseball.fantasysports.yahoo.com/b1/29905/10" xr:uid="{A1CB28C5-E082-4085-AE86-D49CC279CF83}"/>
+    <hyperlink ref="A10" r:id="rId10" display="https://baseball.fantasysports.yahoo.com/b1/29905/11" xr:uid="{D116425B-9BEA-4D21-A5D3-423721F2E905}"/>
+    <hyperlink ref="A11" r:id="rId11" display="https://baseball.fantasysports.yahoo.com/b1/29905/12" xr:uid="{0FD814E4-1AB1-49FD-8354-083F9B5D7F32}"/>
+    <hyperlink ref="A12" r:id="rId12" display="https://baseball.fantasysports.yahoo.com/b1/29905/13" xr:uid="{D60595FD-3831-4281-92F2-13F7D62D6BCE}"/>
+    <hyperlink ref="A13" r:id="rId13" display="https://baseball.fantasysports.yahoo.com/b1/29905/14" xr:uid="{4E38C3B0-7EA6-4F9F-B42E-922FD1456751}"/>
+    <hyperlink ref="A14" r:id="rId14" display="https://baseball.fantasysports.yahoo.com/b1/29905/15" xr:uid="{53E530B9-E473-49DE-991C-87695851E495}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId15"/>
@@ -833,7 +833,7 @@
   <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:G14"/>
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -843,22 +843,22 @@
         <v>1</v>
       </c>
       <c r="B1" s="2">
-        <v>68</v>
+        <v>89</v>
       </c>
       <c r="C1" s="2">
-        <v>1133</v>
+        <v>1557</v>
       </c>
       <c r="D1" s="2">
-        <v>3.92</v>
+        <v>4.18</v>
       </c>
       <c r="E1" s="2">
         <v>1.26</v>
       </c>
       <c r="F1" s="2">
-        <v>82</v>
+        <v>112</v>
       </c>
       <c r="G1" s="2">
-        <v>29</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
@@ -866,22 +866,22 @@
         <v>3</v>
       </c>
       <c r="B2" s="2">
-        <v>77</v>
+        <v>98</v>
       </c>
       <c r="C2" s="2">
-        <v>1122</v>
+        <v>1552</v>
       </c>
       <c r="D2" s="2">
-        <v>4.29</v>
+        <v>4.38</v>
       </c>
       <c r="E2" s="2">
-        <v>1.27</v>
+        <v>1.26</v>
       </c>
       <c r="F2" s="2">
-        <v>73</v>
+        <v>104</v>
       </c>
       <c r="G2" s="2">
-        <v>22</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -889,22 +889,22 @@
         <v>2</v>
       </c>
       <c r="B3" s="2">
-        <v>58</v>
+        <v>78</v>
       </c>
       <c r="C3" s="2">
-        <v>1016</v>
+        <v>1286</v>
       </c>
       <c r="D3" s="2">
-        <v>3.55</v>
+        <v>3.74</v>
       </c>
       <c r="E3" s="2">
-        <v>1.1499999999999999</v>
+        <v>1.19</v>
       </c>
       <c r="F3" s="2">
-        <v>70</v>
+        <v>87</v>
       </c>
       <c r="G3" s="2">
-        <v>31</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="44" thickBot="1" x14ac:dyDescent="0.4">
@@ -912,22 +912,22 @@
         <v>4</v>
       </c>
       <c r="B4" s="2">
-        <v>54</v>
+        <v>75</v>
       </c>
       <c r="C4" s="2">
-        <v>829</v>
+        <v>1184</v>
       </c>
       <c r="D4" s="2">
-        <v>3.35</v>
+        <v>3.34</v>
       </c>
       <c r="E4" s="2">
-        <v>1.08</v>
+        <v>1.0900000000000001</v>
       </c>
       <c r="F4" s="2">
-        <v>45</v>
+        <v>66</v>
       </c>
       <c r="G4" s="2">
-        <v>80</v>
+        <v>103</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
@@ -935,22 +935,22 @@
         <v>5</v>
       </c>
       <c r="B5" s="2">
-        <v>65</v>
+        <v>80</v>
       </c>
       <c r="C5" s="2">
-        <v>1015</v>
+        <v>1352</v>
       </c>
       <c r="D5" s="2">
-        <v>4.38</v>
+        <v>4.45</v>
       </c>
       <c r="E5" s="2">
-        <v>1.27</v>
+        <v>1.29</v>
       </c>
       <c r="F5" s="2">
-        <v>65</v>
+        <v>82</v>
       </c>
       <c r="G5" s="2">
-        <v>33</v>
+        <v>51</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
@@ -958,22 +958,22 @@
         <v>6</v>
       </c>
       <c r="B6" s="2">
-        <v>49</v>
+        <v>73</v>
       </c>
       <c r="C6" s="2">
-        <v>988</v>
+        <v>1357</v>
       </c>
       <c r="D6" s="2">
-        <v>3.87</v>
+        <v>3.81</v>
       </c>
       <c r="E6" s="2">
         <v>1.21</v>
       </c>
       <c r="F6" s="2">
-        <v>58</v>
+        <v>84</v>
       </c>
       <c r="G6" s="2">
-        <v>35</v>
+        <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
@@ -981,22 +981,22 @@
         <v>7</v>
       </c>
       <c r="B7" s="2">
-        <v>61</v>
+        <v>85</v>
       </c>
       <c r="C7" s="2">
-        <v>950</v>
+        <v>1293</v>
       </c>
       <c r="D7" s="2">
-        <v>4.2300000000000004</v>
+        <v>4.51</v>
       </c>
       <c r="E7" s="2">
-        <v>1.28</v>
+        <v>1.3</v>
       </c>
       <c r="F7" s="2">
-        <v>74</v>
+        <v>97</v>
       </c>
       <c r="G7" s="2">
-        <v>-2</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
@@ -1004,22 +1004,22 @@
         <v>0</v>
       </c>
       <c r="B8" s="4">
-        <v>64</v>
+        <v>89</v>
       </c>
       <c r="C8" s="4">
-        <v>1135</v>
+        <v>1554</v>
       </c>
       <c r="D8" s="4">
-        <v>3.83</v>
+        <v>4.04</v>
       </c>
       <c r="E8" s="4">
-        <v>1.19</v>
+        <v>1.22</v>
       </c>
       <c r="F8" s="4">
-        <v>75</v>
+        <v>100</v>
       </c>
       <c r="G8" s="4">
-        <v>24</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
@@ -1027,22 +1027,22 @@
         <v>8</v>
       </c>
       <c r="B9" s="2">
-        <v>73</v>
+        <v>103</v>
       </c>
       <c r="C9" s="2">
-        <v>1141</v>
+        <v>1523</v>
       </c>
       <c r="D9" s="2">
-        <v>3.97</v>
+        <v>4.05</v>
       </c>
       <c r="E9" s="2">
-        <v>1.2</v>
+        <v>1.22</v>
       </c>
       <c r="F9" s="2">
-        <v>85</v>
+        <v>110</v>
       </c>
       <c r="G9" s="2">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
@@ -1050,22 +1050,22 @@
         <v>9</v>
       </c>
       <c r="B10" s="2">
-        <v>66</v>
+        <v>88</v>
       </c>
       <c r="C10" s="2">
-        <v>1104</v>
+        <v>1486</v>
       </c>
       <c r="D10" s="2">
-        <v>3.91</v>
+        <v>3.99</v>
       </c>
       <c r="E10" s="2">
         <v>1.24</v>
       </c>
       <c r="F10" s="2">
-        <v>67</v>
+        <v>96</v>
       </c>
       <c r="G10" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="58.5" thickBot="1" x14ac:dyDescent="0.4">
@@ -1073,22 +1073,22 @@
         <v>10</v>
       </c>
       <c r="B11" s="2">
-        <v>55</v>
+        <v>83</v>
       </c>
       <c r="C11" s="2">
-        <v>985</v>
+        <v>1356</v>
       </c>
       <c r="D11" s="2">
-        <v>3.56</v>
+        <v>3.86</v>
       </c>
       <c r="E11" s="2">
-        <v>1.1599999999999999</v>
+        <v>1.22</v>
       </c>
       <c r="F11" s="2">
-        <v>60</v>
+        <v>81</v>
       </c>
       <c r="G11" s="2">
-        <v>29</v>
+        <v>35</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
@@ -1096,22 +1096,22 @@
         <v>11</v>
       </c>
       <c r="B12" s="2">
-        <v>65</v>
+        <v>82</v>
       </c>
       <c r="C12" s="2">
-        <v>1146</v>
+        <v>1464</v>
       </c>
       <c r="D12" s="2">
-        <v>3.64</v>
+        <v>3.86</v>
       </c>
       <c r="E12" s="2">
-        <v>1.18</v>
+        <v>1.21</v>
       </c>
       <c r="F12" s="2">
-        <v>66</v>
+        <v>82</v>
       </c>
       <c r="G12" s="2">
-        <v>27</v>
+        <v>37</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -1119,22 +1119,22 @@
         <v>12</v>
       </c>
       <c r="B13" s="2">
-        <v>48</v>
+        <v>70</v>
       </c>
       <c r="C13" s="2">
-        <v>685</v>
+        <v>925</v>
       </c>
       <c r="D13" s="2">
-        <v>4.4400000000000004</v>
+        <v>4.42</v>
       </c>
       <c r="E13" s="2">
-        <v>1.38</v>
+        <v>1.35</v>
       </c>
       <c r="F13" s="2">
-        <v>39</v>
+        <v>61</v>
       </c>
       <c r="G13" s="2">
-        <v>27</v>
+        <v>35</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
@@ -1142,41 +1142,42 @@
         <v>13</v>
       </c>
       <c r="B14" s="2">
-        <v>77</v>
+        <v>99</v>
       </c>
       <c r="C14" s="2">
-        <v>997</v>
+        <v>1337</v>
       </c>
       <c r="D14" s="2">
-        <v>3.56</v>
+        <v>3.72</v>
       </c>
       <c r="E14" s="2">
-        <v>1.1599999999999999</v>
+        <v>1.19</v>
       </c>
       <c r="F14" s="2">
-        <v>64</v>
+        <v>89</v>
       </c>
       <c r="G14" s="2">
-        <v>42</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A1" r:id="rId1" display="https://baseball.fantasysports.yahoo.com/b1/29905/1" xr:uid="{34A97C71-F420-4088-A0DD-20C3229FF464}"/>
-    <hyperlink ref="A2" r:id="rId2" display="https://baseball.fantasysports.yahoo.com/b1/29905/3" xr:uid="{516A0371-63DC-4435-B3D0-1642059B66A4}"/>
-    <hyperlink ref="A3" r:id="rId3" display="https://baseball.fantasysports.yahoo.com/b1/29905/4" xr:uid="{496B14C8-1AD0-429C-B692-CF919842A8E5}"/>
-    <hyperlink ref="A4" r:id="rId4" display="https://baseball.fantasysports.yahoo.com/b1/29905/5" xr:uid="{A66F5148-227C-4A83-B780-350ED1F1B401}"/>
-    <hyperlink ref="A5" r:id="rId5" display="https://baseball.fantasysports.yahoo.com/b1/29905/6" xr:uid="{55587CAC-65F7-4E2C-BA4F-39B7304CB319}"/>
-    <hyperlink ref="A6" r:id="rId6" display="https://baseball.fantasysports.yahoo.com/b1/29905/7" xr:uid="{660BEF5D-F094-47FF-862F-EDE2896711D7}"/>
-    <hyperlink ref="A7" r:id="rId7" display="https://baseball.fantasysports.yahoo.com/b1/29905/8" xr:uid="{490B688A-73BD-4C46-8FE2-BD378B4ABED9}"/>
-    <hyperlink ref="A8" r:id="rId8" display="https://baseball.fantasysports.yahoo.com/b1/29905/9" xr:uid="{2FC6355B-2DF9-418F-9DCB-DF8D747F0296}"/>
-    <hyperlink ref="A9" r:id="rId9" display="https://baseball.fantasysports.yahoo.com/b1/29905/10" xr:uid="{DD50C01C-1F64-43CF-9060-36D8A0A72DD5}"/>
-    <hyperlink ref="A10" r:id="rId10" display="https://baseball.fantasysports.yahoo.com/b1/29905/11" xr:uid="{7B5F3BED-4C3D-42FD-B498-66E315B9AE9F}"/>
-    <hyperlink ref="A11" r:id="rId11" display="https://baseball.fantasysports.yahoo.com/b1/29905/12" xr:uid="{A8D32300-282D-4D96-8D97-9666A66233A2}"/>
-    <hyperlink ref="A12" r:id="rId12" display="https://baseball.fantasysports.yahoo.com/b1/29905/13" xr:uid="{5CF9C555-6C2F-43B2-B834-65E0405B07E1}"/>
-    <hyperlink ref="A13" r:id="rId13" display="https://baseball.fantasysports.yahoo.com/b1/29905/14" xr:uid="{BCA24F39-D6FC-4589-9D76-1152D476484B}"/>
-    <hyperlink ref="A14" r:id="rId14" display="https://baseball.fantasysports.yahoo.com/b1/29905/15" xr:uid="{4AD8C469-237A-4B75-8997-E8103145E461}"/>
+    <hyperlink ref="A1" r:id="rId1" display="https://baseball.fantasysports.yahoo.com/b1/29905/1" xr:uid="{B9258295-4992-482E-8835-223F78C635AF}"/>
+    <hyperlink ref="A2" r:id="rId2" display="https://baseball.fantasysports.yahoo.com/b1/29905/3" xr:uid="{ECF4050E-7D54-4860-B5C6-DADAE28CAC4D}"/>
+    <hyperlink ref="A3" r:id="rId3" display="https://baseball.fantasysports.yahoo.com/b1/29905/4" xr:uid="{402C7C93-979B-4A4D-BD6B-D94F7C9F324C}"/>
+    <hyperlink ref="A4" r:id="rId4" display="https://baseball.fantasysports.yahoo.com/b1/29905/5" xr:uid="{961F516F-0C38-4DDF-9AEF-2A68BB6D42E0}"/>
+    <hyperlink ref="A5" r:id="rId5" display="https://baseball.fantasysports.yahoo.com/b1/29905/6" xr:uid="{C5C18A8D-67FC-4D73-ADC3-5D03E8BCDB32}"/>
+    <hyperlink ref="A6" r:id="rId6" display="https://baseball.fantasysports.yahoo.com/b1/29905/7" xr:uid="{8803FC8D-B3FB-4601-A60A-C2D8BDBFCD5C}"/>
+    <hyperlink ref="A7" r:id="rId7" display="https://baseball.fantasysports.yahoo.com/b1/29905/8" xr:uid="{9096EE09-1318-4F7E-92F7-4692001EBC94}"/>
+    <hyperlink ref="A8" r:id="rId8" display="https://baseball.fantasysports.yahoo.com/b1/29905/9" xr:uid="{C5D4D405-A7FD-4070-B112-FEE54732E0F5}"/>
+    <hyperlink ref="A9" r:id="rId9" display="https://baseball.fantasysports.yahoo.com/b1/29905/10" xr:uid="{AC067905-0C5A-4364-899C-6E864A2503BB}"/>
+    <hyperlink ref="A10" r:id="rId10" display="https://baseball.fantasysports.yahoo.com/b1/29905/11" xr:uid="{EF22D1B7-1A93-42AF-8EF4-950A676B23B1}"/>
+    <hyperlink ref="A11" r:id="rId11" display="https://baseball.fantasysports.yahoo.com/b1/29905/12" xr:uid="{C370E696-4400-4005-A982-3A4D66B960A8}"/>
+    <hyperlink ref="A12" r:id="rId12" display="https://baseball.fantasysports.yahoo.com/b1/29905/13" xr:uid="{174B2323-A837-43FE-96A9-537FCAD26910}"/>
+    <hyperlink ref="A13" r:id="rId13" display="https://baseball.fantasysports.yahoo.com/b1/29905/14" xr:uid="{8C97A1C1-15C3-43CA-A8CC-9A48C99F1A0E}"/>
+    <hyperlink ref="A14" r:id="rId14" display="https://baseball.fantasysports.yahoo.com/b1/29905/15" xr:uid="{10373002-46EC-4177-9630-111899F0F8EB}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId15"/>
 </worksheet>
 </file>
</xml_diff>